<commit_message>
Se hace ajuste en api de GetResultadosMuestreoEstatusMuestreoAsync para obtener el costo de parametro Se agrega columnas de "Validación final" y "Observaciones final" en archivo que se descarag en la pantalla de Resumen reglas Se agrega propiedad de resultadoReglas en interface de acumuladosMuestreo Se agrega filtro en pantalla de Liberacion se ajusta frnt botones y columnas tambien se agrega componente de ventana emergente y notificaciones Se agregan columna en panatlal de incio de reglas para validacion automatica de si se debe o no correr la regla de validacion Validacion para aplicacion de reglas en modulo de reglas Ajuste de front de columnas en pantalla resumen reglas
</commit_message>
<xml_diff>
--- a/WebAPI/wwwroot/Plantillas/ResumenReglasValidacionResultado.xlsx
+++ b/WebAPI/wwwroot/Plantillas/ResumenReglasValidacionResultado.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16395" windowHeight="4290"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16392" windowHeight="4296"/>
   </bookViews>
   <sheets>
     <sheet name="ResumenValidacionReglas_Resulta" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Clave Unica</t>
   </si>
@@ -114,6 +114,12 @@
   </si>
   <si>
     <t>Número entrega</t>
+  </si>
+  <si>
+    <t>Validación final</t>
+  </si>
+  <si>
+    <t>Observaciones final</t>
   </si>
 </sst>
 </file>
@@ -135,7 +141,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,6 +166,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -173,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -197,6 +209,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -479,17 +494,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD1"/>
+  <dimension ref="A1:AF1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AF10" sqref="AF10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="28" max="28" width="12.5703125" customWidth="1"/>
-    <col min="29" max="29" width="14.85546875" customWidth="1"/>
+    <col min="28" max="28" width="12.5546875" customWidth="1"/>
+    <col min="29" max="29" width="14.88671875" customWidth="1"/>
+    <col min="32" max="32" width="13.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>29</v>
       </c>
@@ -579,6 +597,12 @@
       </c>
       <c r="AD1" s="7" t="s">
         <v>28</v>
+      </c>
+      <c r="AE1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="9" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>